<commit_message>
More stations and updated sheets
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1820sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1820sLOCATIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99421D0-FAEF-BF45-9D1D-5EFCF143C6BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BCF777-1860-8444-A030-421E9184F7C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="591">
   <si>
     <t>LOCATIONS IN 1820s onwards</t>
   </si>
@@ -2164,6 +2164,9 @@
   </si>
   <si>
     <t>RR237</t>
+  </si>
+  <si>
+    <t>RR261</t>
   </si>
 </sst>
 </file>
@@ -2767,8 +2770,8 @@
   <dimension ref="A1:AB1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <pane ySplit="6" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7803,6 +7806,9 @@
       </c>
       <c r="G201" s="28">
         <v>1830</v>
+      </c>
+      <c r="H201" s="47" t="s">
+        <v>590</v>
       </c>
       <c r="K201" s="27" t="s">
         <v>460</v>

</xml_diff>

<commit_message>
Further locations added and location sheets updated
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1820sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1820sLOCATIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BCF777-1860-8444-A030-421E9184F7C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1DCEB5-66B7-B245-88BA-33C9DC74F9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2769,9 +2769,9 @@
   </sheetPr>
   <dimension ref="A1:AB1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H201" sqref="H201"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I177" sqref="I177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -4723,6 +4723,9 @@
       <c r="G79" s="28">
         <v>1820</v>
       </c>
+      <c r="H79">
+        <v>3602</v>
+      </c>
       <c r="K79" s="27" t="s">
         <v>194</v>
       </c>
@@ -7132,6 +7135,9 @@
       </c>
       <c r="G173" s="28">
         <v>1830</v>
+      </c>
+      <c r="H173">
+        <v>3602</v>
       </c>
       <c r="I173" s="36" t="s">
         <v>193</v>

</xml_diff>